<commit_message>
chore: fix image fields in db tables, add folder with images
</commit_message>
<xml_diff>
--- a/docs/data_dictionary.xlsx
+++ b/docs/data_dictionary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59626A99-394A-407A-8ADA-7D0DE1EEF1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFA9EF3-92EF-4864-A793-17B0563C719F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11316" yWindow="348" windowWidth="12072" windowHeight="11436" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataDictionary" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="82">
   <si>
     <t>Data Dictionary</t>
   </si>
@@ -835,10 +835,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E90"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1108,79 +1108,77 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="72">
-      <c r="A21" s="8" t="s">
-        <v>35</v>
-      </c>
+    <row r="21" spans="1:5">
+      <c r="A21" s="8"/>
       <c r="B21" s="9" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="72">
+      <c r="A22" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A23" s="21" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="10"/>
+    </row>
+    <row r="24" spans="1:5" ht="21.75" customHeight="1">
+      <c r="A24" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-    </row>
-    <row r="24" spans="1:5" ht="27.6" customHeight="1">
-      <c r="A24" s="11" t="s">
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+    </row>
+    <row r="25" spans="1:5" ht="27.6" customHeight="1">
+      <c r="A25" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B25" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="E25" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="8" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B26" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="57.6">
-      <c r="A26" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>24</v>
@@ -1188,118 +1186,118 @@
       <c r="D26" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="57.6">
+      <c r="A27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="8"/>
-      <c r="B27" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" ht="57.6">
+    <row r="28" spans="1:5">
       <c r="A28" s="8"/>
       <c r="B28" s="9" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="28.8">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="57.6">
       <c r="A29" s="8"/>
       <c r="B29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="28.8">
+      <c r="A30" s="8"/>
+      <c r="B30" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C30" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="D30" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A30" s="8" t="s">
+    <row r="31" spans="1:5" ht="21.75" customHeight="1">
+      <c r="A31" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B31" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C31" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="D31" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="20.25" customHeight="1">
-      <c r="A31" s="14"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="21" t="s">
+    <row r="32" spans="1:5" ht="20.25" customHeight="1">
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-    </row>
-    <row r="33" spans="1:5" ht="28.8">
-      <c r="A33" s="11" t="s">
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+    </row>
+    <row r="34" spans="1:5" ht="28.8">
+      <c r="A34" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B34" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C34" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="11" t="s">
+      <c r="D34" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E34" s="12" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1307,175 +1305,175 @@
         <v>9</v>
       </c>
       <c r="B35" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C36" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="2" t="s">
+      <c r="D36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A37" s="21" t="s">
+    <row r="38" spans="1:5" ht="21.75" customHeight="1">
+      <c r="A38" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-    </row>
-    <row r="38" spans="1:5" ht="31.2" customHeight="1">
-      <c r="A38" s="11" t="s">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+    </row>
+    <row r="39" spans="1:5" ht="31.2" customHeight="1">
+      <c r="A39" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B39" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C39" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E39" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="8" t="s">
+    <row r="40" spans="1:5">
+      <c r="A40" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B40" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C40" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D39" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="18" t="s">
+      <c r="D40" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="18"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="8"/>
       <c r="B41" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="17" t="s">
         <v>26</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="E41" s="18"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="8"/>
       <c r="B42" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="8"/>
+      <c r="B43" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="8" t="s">
+      <c r="D43" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B44" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="D44" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="8"/>
-      <c r="B44" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="8"/>
       <c r="B45" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E45" s="2"/>
+      <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="8"/>
       <c r="B46" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>26</v>
       </c>
       <c r="D46" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="8"/>
+      <c r="B47" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1483,185 +1481,185 @@
         <v>35</v>
       </c>
       <c r="B48" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C49" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" s="3" t="s">
+      <c r="D49" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="21" t="s">
+    <row r="51" spans="1:5">
+      <c r="A51" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-    </row>
-    <row r="51" spans="1:5" ht="28.8">
-      <c r="A51" s="11" t="s">
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+    </row>
+    <row r="52" spans="1:5" ht="28.8">
+      <c r="A52" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B52" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C52" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D52" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="12" t="s">
+      <c r="E52" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="8" t="s">
+    <row r="53" spans="1:5">
+      <c r="A53" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B53" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C53" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D52" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="18" t="s">
+      <c r="D53" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="8"/>
-      <c r="B53" s="9" t="s">
+    <row r="54" spans="1:5">
+      <c r="A54" s="8"/>
+      <c r="B54" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C54" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D53" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" s="3" t="s">
+      <c r="D54" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="21" t="s">
+    <row r="56" spans="1:5">
+      <c r="A56" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-    </row>
-    <row r="56" spans="1:5" ht="28.8">
-      <c r="A56" s="11" t="s">
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+    </row>
+    <row r="57" spans="1:5" ht="28.8">
+      <c r="A57" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B57" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C57" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D56" s="11" t="s">
+      <c r="D57" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E56" s="12" t="s">
+      <c r="E57" s="12" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B59" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D58" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" s="2" t="s">
+      <c r="D59" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="21" t="s">
+    <row r="61" spans="1:5">
+      <c r="A61" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B60" s="21"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-    </row>
-    <row r="61" spans="1:5" ht="28.8">
-      <c r="A61" s="11" t="s">
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+    </row>
+    <row r="62" spans="1:5" ht="28.8">
+      <c r="A62" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B62" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C62" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D62" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E62" s="12" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="8" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C63" s="17" t="s">
         <v>24</v>
@@ -1670,7 +1668,7 @@
         <v>7</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1678,7 +1676,7 @@
         <v>10</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C64" s="17" t="s">
         <v>24</v>
@@ -1687,50 +1685,50 @@
         <v>7</v>
       </c>
       <c r="E64" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="21" t="s">
+    <row r="67" spans="1:5">
+      <c r="A67" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B66" s="21"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-    </row>
-    <row r="67" spans="1:5" ht="28.8">
-      <c r="A67" s="11" t="s">
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+    </row>
+    <row r="68" spans="1:5" ht="28.8">
+      <c r="A68" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B67" s="12" t="s">
+      <c r="B68" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C67" s="12" t="s">
+      <c r="C68" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D68" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E67" s="12" t="s">
+      <c r="E68" s="12" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1738,80 +1736,82 @@
         <v>66</v>
       </c>
       <c r="B69" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D69" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E69" s="2" t="s">
+      <c r="D70" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="21" t="s">
+    <row r="72" spans="1:5">
+      <c r="A72" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B71" s="21"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
-      <c r="E71" s="21"/>
-    </row>
-    <row r="72" spans="1:5" ht="28.8">
-      <c r="A72" s="11" t="s">
+      <c r="B72" s="21"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+    </row>
+    <row r="73" spans="1:5" ht="28.8">
+      <c r="A73" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B72" s="12" t="s">
+      <c r="B73" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C73" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D72" s="11" t="s">
+      <c r="D73" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E73" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
-      <c r="A73" s="8" t="s">
+    <row r="74" spans="1:5">
+      <c r="A74" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B74" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D73" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E73" s="18" t="s">
+      <c r="D74" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="18" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="28.8">
-      <c r="A74" s="8"/>
-      <c r="B74" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="28.8">
       <c r="A75" s="8"/>
       <c r="B75" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>26</v>
@@ -1820,13 +1820,13 @@
         <v>7</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="28.8">
       <c r="A76" s="8"/>
       <c r="B76" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>26</v>
@@ -1835,131 +1835,129 @@
         <v>7</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="28.8">
       <c r="A77" s="8"/>
       <c r="B77" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="28.8">
+      <c r="A78" s="8"/>
+      <c r="B78" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="19" t="s">
+      <c r="C78" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D77" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E77" s="1" t="s">
+      <c r="D78" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="21" t="s">
+    <row r="80" spans="1:5">
+      <c r="A80" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B79" s="21"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
-    </row>
-    <row r="80" spans="1:5" ht="28.8">
-      <c r="A80" s="11" t="s">
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+    </row>
+    <row r="81" spans="1:5" ht="28.8">
+      <c r="A81" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B80" s="12" t="s">
+      <c r="B81" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C80" s="12" t="s">
+      <c r="C81" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D80" s="11" t="s">
+      <c r="D81" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E80" s="12" t="s">
+      <c r="E81" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
-      <c r="A81" s="8" t="s">
+    <row r="82" spans="1:5">
+      <c r="A82" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B82" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C82" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D81" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E81" s="18" t="s">
+      <c r="D82" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E82" s="18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
-      <c r="A82" s="8"/>
-      <c r="B82" s="9" t="s">
+    <row r="83" spans="1:5">
+      <c r="A83" s="8"/>
+      <c r="B83" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D82" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E82" s="1" t="s">
+      <c r="D83" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="21" t="s">
+    <row r="85" spans="1:5">
+      <c r="A85" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B84" s="21"/>
-      <c r="C84" s="21"/>
-      <c r="D84" s="21"/>
-      <c r="E84" s="21"/>
-    </row>
-    <row r="85" spans="1:5" ht="28.8">
-      <c r="A85" s="11" t="s">
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="21"/>
+      <c r="E85" s="21"/>
+    </row>
+    <row r="86" spans="1:5" ht="28.8">
+      <c r="A86" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B86" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C85" s="12" t="s">
+      <c r="C86" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D85" s="11" t="s">
+      <c r="D86" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E85" s="12" t="s">
+      <c r="E86" s="12" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E86" s="18" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>24</v>
@@ -1967,49 +1965,66 @@
       <c r="D87" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="E87" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
-      <c r="A88" s="8"/>
-      <c r="B88" s="9" t="s">
+    <row r="89" spans="1:5">
+      <c r="A89" s="8"/>
+      <c r="B89" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C88" s="17" t="s">
+      <c r="C89" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D88" s="8" t="s">
+      <c r="D89" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E89" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
-      <c r="A89" s="5"/>
-      <c r="D89" s="5"/>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="5"/>
       <c r="D90" s="5"/>
     </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="5"/>
+      <c r="D91" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A66:E66"/>
-    <mergeCell ref="A71:E71"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="A84:E84"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A60:E60"/>
-    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="A33:E33"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A24:E24"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="A72:E72"/>
+    <mergeCell ref="A80:E80"/>
+    <mergeCell ref="A85:E85"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="A61:E61"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.2" right="0.2" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>

</xml_diff>